<commit_message>
finish up till 35
</commit_message>
<xml_diff>
--- a/cleaned_data/Meta_data_demo.xlsx
+++ b/cleaned_data/Meta_data_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC374BE5-4FA7-4CE8-8905-084A5FE471BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE3D33D-60F7-4196-BCB8-FB9AABEF03D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,27 +496,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK31"/>
+  <dimension ref="A1:AK51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AK50" sqref="AK50:AK51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="8.7265625" style="3"/>
-    <col min="6" max="8" width="8.81640625" customWidth="1"/>
-    <col min="9" max="9" width="8.81640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" style="3"/>
-    <col min="17" max="17" width="8.7265625" style="3"/>
-    <col min="21" max="21" width="8.7265625" style="3"/>
-    <col min="25" max="25" width="8.7265625" style="3"/>
-    <col min="29" max="29" width="8.7265625" style="3"/>
-    <col min="33" max="33" width="8.7265625" style="3"/>
-    <col min="37" max="37" width="8.7265625" style="3"/>
+    <col min="5" max="5" width="8.7109375" style="3"/>
+    <col min="6" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="3"/>
+    <col min="17" max="17" width="8.7109375" style="3"/>
+    <col min="21" max="21" width="8.7109375" style="3"/>
+    <col min="25" max="25" width="8.7109375" style="3"/>
+    <col min="29" max="29" width="8.7109375" style="3"/>
+    <col min="33" max="33" width="8.7109375" style="3"/>
+    <col min="37" max="37" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +632,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -670,7 +673,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -681,43 +684,43 @@
         <v>165</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E31" si="0">IF(SUM(B3:D3)=0,"NA",SUM(B3:D3))</f>
+        <f t="shared" ref="E3:E51" si="0">IF(SUM(B3:D3)=0,"NA",SUM(B3:D3))</f>
         <v>400</v>
       </c>
       <c r="I3" s="3" t="str">
-        <f t="shared" ref="I3:I31" si="1">IF(SUM(F3:H3)=0,"NA",SUM(F3:H3))</f>
+        <f t="shared" ref="I3:I51" si="1">IF(SUM(F3:H3)=0,"NA",SUM(F3:H3))</f>
         <v>NA</v>
       </c>
       <c r="M3" s="3" t="str">
-        <f t="shared" ref="M3:M31" si="2">IF(SUM(J3:L3)=0,"NA",SUM(J3:L3))</f>
+        <f t="shared" ref="M3:M51" si="2">IF(SUM(J3:L3)=0,"NA",SUM(J3:L3))</f>
         <v>NA</v>
       </c>
       <c r="Q3" s="3" t="str">
-        <f t="shared" ref="Q3:Q31" si="3">IF(SUM(N3:P3)=0,"NA",SUM(N3:P3))</f>
+        <f t="shared" ref="Q3:Q51" si="3">IF(SUM(N3:P3)=0,"NA",SUM(N3:P3))</f>
         <v>NA</v>
       </c>
       <c r="U3" s="3" t="str">
-        <f t="shared" ref="U3:U31" si="4">IF(SUM(R3:T3)=0,"NA",SUM(R3:T3))</f>
+        <f t="shared" ref="U3:U51" si="4">IF(SUM(R3:T3)=0,"NA",SUM(R3:T3))</f>
         <v>NA</v>
       </c>
       <c r="Y3" s="3" t="str">
-        <f t="shared" ref="Y3:Y31" si="5">IF(SUM(V3:X3)=0,"NA",SUM(V3:X3))</f>
+        <f t="shared" ref="Y3:Y51" si="5">IF(SUM(V3:X3)=0,"NA",SUM(V3:X3))</f>
         <v>NA</v>
       </c>
       <c r="AC3" s="3" t="str">
-        <f t="shared" ref="AC3:AC31" si="6">IF(SUM(Z3:AB3)=0,"NA",SUM(Z3:AB3))</f>
+        <f t="shared" ref="AC3:AC51" si="6">IF(SUM(Z3:AB3)=0,"NA",SUM(Z3:AB3))</f>
         <v>NA</v>
       </c>
       <c r="AG3" s="3" t="str">
-        <f t="shared" ref="AG3:AG31" si="7">IF(SUM(AD3:AF3)=0,"NA",SUM(AD3:AF3))</f>
+        <f t="shared" ref="AG3:AG51" si="7">IF(SUM(AD3:AF3)=0,"NA",SUM(AD3:AF3))</f>
         <v>NA</v>
       </c>
       <c r="AK3" s="3" t="str">
-        <f t="shared" ref="AK3:AK31" si="8">IF(SUM(AH3:AJ3)=0,"NA",SUM(AH3:AJ3))</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+        <f t="shared" ref="AK3:AK51" si="8">IF(SUM(AH3:AJ3)=0,"NA",SUM(AH3:AJ3))</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -782,7 +785,7 @@
         <v>5410</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -829,7 +832,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -876,7 +879,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -923,7 +926,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -988,7 +991,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1308,7 +1311,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1490,7 +1493,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1674,7 +1677,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1959,7 +1962,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2043,6 +2046,880 @@
         <v>NA</v>
       </c>
       <c r="AK31" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>301</v>
+      </c>
+      <c r="C32">
+        <v>456</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="0"/>
+        <v>757</v>
+      </c>
+      <c r="I32" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M32" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q32" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U32" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y32" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC32" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG32" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK32" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>170</v>
+      </c>
+      <c r="C33">
+        <v>141</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="0"/>
+        <v>311</v>
+      </c>
+      <c r="I33" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M33" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q33" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U33" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y33" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC33" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG33" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK33" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>67</v>
+      </c>
+      <c r="C34">
+        <v>87</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+      <c r="I34" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="M34" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N34">
+        <v>2</v>
+      </c>
+      <c r="O34">
+        <v>5</v>
+      </c>
+      <c r="Q34" s="3">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="U34" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="V34">
+        <v>62</v>
+      </c>
+      <c r="W34">
+        <v>77</v>
+      </c>
+      <c r="Y34" s="3">
+        <f t="shared" si="5"/>
+        <v>139</v>
+      </c>
+      <c r="Z34">
+        <v>2</v>
+      </c>
+      <c r="AA34">
+        <v>4</v>
+      </c>
+      <c r="AC34" s="3">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AD34">
+        <v>1</v>
+      </c>
+      <c r="AE34">
+        <v>7</v>
+      </c>
+      <c r="AG34" s="3">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AH34">
+        <v>66</v>
+      </c>
+      <c r="AI34">
+        <v>80</v>
+      </c>
+      <c r="AK34" s="3">
+        <f t="shared" si="8"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="E35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I35" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M35" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q35" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U35" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y35" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC35" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG35" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK35" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="E36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I36" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M36" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q36" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U36" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y36" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC36" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG36" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK36" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="E37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I37" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M37" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q37" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U37" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y37" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC37" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG37" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK37" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="E38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I38" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M38" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q38" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U38" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y38" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC38" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG38" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK38" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="E39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I39" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M39" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q39" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U39" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y39" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC39" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG39" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK39" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="E40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I40" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M40" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q40" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U40" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y40" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC40" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG40" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK40" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="E41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I41" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M41" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q41" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U41" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y41" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC41" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG41" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK41" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="E42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I42" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M42" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q42" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U42" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y42" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC42" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG42" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK42" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="E43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I43" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M43" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q43" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U43" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y43" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC43" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG43" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK43" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="E44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I44" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M44" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q44" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U44" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y44" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC44" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG44" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK44" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="E45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I45" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M45" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q45" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U45" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y45" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC45" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG45" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK45" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="E46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I46" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M46" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q46" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U46" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y46" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC46" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG46" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK46" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="E47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I47" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M47" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q47" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U47" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y47" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC47" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG47" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK47" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="E48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I48" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M48" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q48" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U48" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y48" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC48" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG48" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK48" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="E49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I49" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M49" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q49" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U49" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y49" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC49" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG49" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK49" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="E50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I50" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M50" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q50" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U50" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y50" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC50" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG50" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK50" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="E51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I51" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="M51" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="Q51" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="U51" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="Y51" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="AC51" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="AG51" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="AK51" s="3" t="str">
         <f t="shared" si="8"/>
         <v>NA</v>
       </c>

</xml_diff>

<commit_message>
complete up till 45
</commit_message>
<xml_diff>
--- a/cleaned_data/Meta_data_demo.xlsx
+++ b/cleaned_data/Meta_data_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2002798B-DFEF-41B5-9EEE-BBCC2054746C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048F2D89-59B5-48B2-937F-C55F22BF31B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,10 +499,10 @@
   <dimension ref="A1:AK51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I49" sqref="I49"/>
+      <selection pane="bottomRight" activeCell="AA50" sqref="AA50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2706,9 +2706,15 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="E45" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="B45">
+        <v>55</v>
+      </c>
+      <c r="C45">
+        <v>72</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="0"/>
+        <v>127</v>
       </c>
       <c r="I45" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2747,41 +2753,65 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="E46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="B46">
+        <v>25</v>
+      </c>
+      <c r="C46">
+        <v>39</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="0"/>
+        <v>64</v>
       </c>
       <c r="I46" s="3" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="M46" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>NA</v>
-      </c>
-      <c r="Q46" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
+      <c r="L46">
+        <v>4</v>
+      </c>
+      <c r="M46" s="3">
+        <f>IF(SUM(J46:L46)=0,"NA",SUM(J46:L46))</f>
+        <v>4</v>
+      </c>
+      <c r="P46">
+        <v>12</v>
+      </c>
+      <c r="Q46" s="3">
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
       <c r="U46" s="3" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="Y46" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>NA</v>
-      </c>
-      <c r="AC46" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG46" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-      <c r="AK46" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>NA</v>
+      <c r="X46">
+        <v>34</v>
+      </c>
+      <c r="Y46" s="3">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="AB46">
+        <v>5</v>
+      </c>
+      <c r="AC46" s="3">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AF46">
+        <v>9</v>
+      </c>
+      <c r="AG46" s="3">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="AJ46">
+        <v>50</v>
+      </c>
+      <c r="AK46" s="3">
+        <f t="shared" si="8"/>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finish up till 47
</commit_message>
<xml_diff>
--- a/cleaned_data/Meta_data_demo.xlsx
+++ b/cleaned_data/Meta_data_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048F2D89-59B5-48B2-937F-C55F22BF31B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34F32B9-84CB-4A5A-BDFB-75C0A1856BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,10 +499,10 @@
   <dimension ref="A1:AK51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA50" sqref="AA50"/>
+      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,9 +2818,15 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="E47" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="B47">
+        <v>26</v>
+      </c>
+      <c r="C47">
+        <v>44</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="0"/>
+        <v>70</v>
       </c>
       <c r="I47" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2859,9 +2865,16 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="E48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="B48">
+        <f>252-93</f>
+        <v>159</v>
+      </c>
+      <c r="C48">
+        <v>93</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="0"/>
+        <v>252</v>
       </c>
       <c r="I48" s="3" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
complete all 50 trials
</commit_message>
<xml_diff>
--- a/cleaned_data/Meta_data_demo.xlsx
+++ b/cleaned_data/Meta_data_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34F32B9-84CB-4A5A-BDFB-75C0A1856BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC55789-AF40-45F2-AB38-0993E6511356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,10 +499,10 @@
   <dimension ref="A1:AK51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,9 +2913,15 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="E49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="B49">
+        <v>375</v>
+      </c>
+      <c r="C49">
+        <v>384</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="0"/>
+        <v>759</v>
       </c>
       <c r="I49" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2954,9 +2960,15 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="E50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="B50">
+        <v>37</v>
+      </c>
+      <c r="C50">
+        <v>37</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="0"/>
+        <v>74</v>
       </c>
       <c r="I50" s="3" t="str">
         <f t="shared" si="1"/>
@@ -2995,9 +3007,15 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="E51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="B51">
+        <v>76</v>
+      </c>
+      <c r="C51">
+        <v>161</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="0"/>
+        <v>237</v>
       </c>
       <c r="I51" s="3" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
update, only missing 48 and 50
</commit_message>
<xml_diff>
--- a/cleaned_data/Meta_data_demo.xlsx
+++ b/cleaned_data/Meta_data_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC55789-AF40-45F2-AB38-0993E6511356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9920CE-336C-487A-B5A4-84871D117911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Trial_ID</t>
   </si>
@@ -147,6 +147,24 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>cluster1</t>
+  </si>
+  <si>
+    <t>cluster6</t>
+  </si>
+  <si>
+    <t>cluster5</t>
+  </si>
+  <si>
+    <t>cluster2</t>
+  </si>
+  <si>
+    <t>cluster3</t>
+  </si>
+  <si>
+    <t>cluster4</t>
   </si>
 </sst>
 </file>
@@ -496,19 +514,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK51"/>
+  <dimension ref="A1:AK57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="8.7109375" style="3"/>
-    <col min="6" max="8" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" style="3"/>
     <col min="17" max="17" width="8.7109375" style="3"/>
@@ -684,39 +704,39 @@
         <v>165</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E51" si="0">IF(SUM(B3:D3)=0,"NA",SUM(B3:D3))</f>
+        <f t="shared" ref="E3:E54" si="0">IF(SUM(B3:D3)=0,"NA",SUM(B3:D3))</f>
         <v>400</v>
       </c>
       <c r="I3" s="3" t="str">
-        <f t="shared" ref="I3:I51" si="1">IF(SUM(F3:H3)=0,"NA",SUM(F3:H3))</f>
+        <f>IF(SUM(F3:H3)=0,"NA",SUM(F3:H3))</f>
         <v>NA</v>
       </c>
       <c r="M3" s="3" t="str">
-        <f t="shared" ref="M3:M51" si="2">IF(SUM(J3:L3)=0,"NA",SUM(J3:L3))</f>
+        <f>IF(SUM(J3:L3)=0,"NA",SUM(J3:L3))</f>
         <v>NA</v>
       </c>
       <c r="Q3" s="3" t="str">
-        <f t="shared" ref="Q3:Q51" si="3">IF(SUM(N3:P3)=0,"NA",SUM(N3:P3))</f>
+        <f>IF(SUM(N3:P3)=0,"NA",SUM(N3:P3))</f>
         <v>NA</v>
       </c>
       <c r="U3" s="3" t="str">
-        <f t="shared" ref="U3:U51" si="4">IF(SUM(R3:T3)=0,"NA",SUM(R3:T3))</f>
+        <f>IF(SUM(R3:T3)=0,"NA",SUM(R3:T3))</f>
         <v>NA</v>
       </c>
       <c r="Y3" s="3" t="str">
-        <f t="shared" ref="Y3:Y51" si="5">IF(SUM(V3:X3)=0,"NA",SUM(V3:X3))</f>
+        <f>IF(SUM(V3:X3)=0,"NA",SUM(V3:X3))</f>
         <v>NA</v>
       </c>
       <c r="AC3" s="3" t="str">
-        <f t="shared" ref="AC3:AC51" si="6">IF(SUM(Z3:AB3)=0,"NA",SUM(Z3:AB3))</f>
+        <f>IF(SUM(Z3:AB3)=0,"NA",SUM(Z3:AB3))</f>
         <v>NA</v>
       </c>
       <c r="AG3" s="3" t="str">
-        <f t="shared" ref="AG3:AG51" si="7">IF(SUM(AD3:AF3)=0,"NA",SUM(AD3:AF3))</f>
+        <f>IF(SUM(AD3:AF3)=0,"NA",SUM(AD3:AF3))</f>
         <v>NA</v>
       </c>
       <c r="AK3" s="3" t="str">
-        <f t="shared" ref="AK3:AK51" si="8">IF(SUM(AH3:AJ3)=0,"NA",SUM(AH3:AJ3))</f>
+        <f>IF(SUM(AH3:AJ3)=0,"NA",SUM(AH3:AJ3))</f>
         <v>NA</v>
       </c>
     </row>
@@ -735,11 +755,11 @@
         <v>5536</v>
       </c>
       <c r="I4" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F4:H4)=0,"NA",SUM(F4:H4))</f>
         <v>NA</v>
       </c>
       <c r="M4" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(J4:L4)=0,"NA",SUM(J4:L4))</f>
         <v>NA</v>
       </c>
       <c r="N4">
@@ -749,19 +769,19 @@
         <v>494</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="3"/>
+        <f>IF(SUM(N4:P4)=0,"NA",SUM(N4:P4))</f>
         <v>946</v>
       </c>
       <c r="U4" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R4:T4)=0,"NA",SUM(R4:T4))</f>
         <v>NA</v>
       </c>
       <c r="Y4" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(SUM(V4:X4)=0,"NA",SUM(V4:X4))</f>
         <v>NA</v>
       </c>
       <c r="AC4" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z4:AB4)=0,"NA",SUM(Z4:AB4))</f>
         <v>NA</v>
       </c>
       <c r="AD4">
@@ -771,7 +791,7 @@
         <v>304</v>
       </c>
       <c r="AG4" s="3">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD4:AF4)=0,"NA",SUM(AD4:AF4))</f>
         <v>620</v>
       </c>
       <c r="AH4">
@@ -781,7 +801,7 @@
         <v>2578</v>
       </c>
       <c r="AK4" s="3">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH4:AJ4)=0,"NA",SUM(AH4:AJ4))</f>
         <v>5410</v>
       </c>
     </row>
@@ -800,35 +820,35 @@
         <v>75</v>
       </c>
       <c r="I5" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F5:H5)=0,"NA",SUM(F5:H5))</f>
         <v>NA</v>
       </c>
       <c r="M5" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(J5:L5)=0,"NA",SUM(J5:L5))</f>
         <v>NA</v>
       </c>
       <c r="Q5" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(SUM(N5:P5)=0,"NA",SUM(N5:P5))</f>
         <v>NA</v>
       </c>
       <c r="U5" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R5:T5)=0,"NA",SUM(R5:T5))</f>
         <v>NA</v>
       </c>
       <c r="Y5" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(SUM(V5:X5)=0,"NA",SUM(V5:X5))</f>
         <v>NA</v>
       </c>
       <c r="AC5" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z5:AB5)=0,"NA",SUM(Z5:AB5))</f>
         <v>NA</v>
       </c>
       <c r="AG5" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD5:AF5)=0,"NA",SUM(AD5:AF5))</f>
         <v>NA</v>
       </c>
       <c r="AK5" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH5:AJ5)=0,"NA",SUM(AH5:AJ5))</f>
         <v>NA</v>
       </c>
     </row>
@@ -847,35 +867,35 @@
         <v>5060</v>
       </c>
       <c r="I6" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F6:H6)=0,"NA",SUM(F6:H6))</f>
         <v>NA</v>
       </c>
       <c r="M6" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(J6:L6)=0,"NA",SUM(J6:L6))</f>
         <v>NA</v>
       </c>
       <c r="Q6" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(SUM(N6:P6)=0,"NA",SUM(N6:P6))</f>
         <v>NA</v>
       </c>
       <c r="U6" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R6:T6)=0,"NA",SUM(R6:T6))</f>
         <v>NA</v>
       </c>
       <c r="Y6" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(SUM(V6:X6)=0,"NA",SUM(V6:X6))</f>
         <v>NA</v>
       </c>
       <c r="AC6" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z6:AB6)=0,"NA",SUM(Z6:AB6))</f>
         <v>NA</v>
       </c>
       <c r="AG6" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD6:AF6)=0,"NA",SUM(AD6:AF6))</f>
         <v>NA</v>
       </c>
       <c r="AK6" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH6:AJ6)=0,"NA",SUM(AH6:AJ6))</f>
         <v>NA</v>
       </c>
     </row>
@@ -894,35 +914,35 @@
         <v>463</v>
       </c>
       <c r="I7" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F7:H7)=0,"NA",SUM(F7:H7))</f>
         <v>NA</v>
       </c>
       <c r="M7" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(J7:L7)=0,"NA",SUM(J7:L7))</f>
         <v>NA</v>
       </c>
       <c r="Q7" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(SUM(N7:P7)=0,"NA",SUM(N7:P7))</f>
         <v>NA</v>
       </c>
       <c r="U7" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R7:T7)=0,"NA",SUM(R7:T7))</f>
         <v>NA</v>
       </c>
       <c r="Y7" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(SUM(V7:X7)=0,"NA",SUM(V7:X7))</f>
         <v>NA</v>
       </c>
       <c r="AC7" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z7:AB7)=0,"NA",SUM(Z7:AB7))</f>
         <v>NA</v>
       </c>
       <c r="AG7" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD7:AF7)=0,"NA",SUM(AD7:AF7))</f>
         <v>NA</v>
       </c>
       <c r="AK7" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH7:AJ7)=0,"NA",SUM(AH7:AJ7))</f>
         <v>NA</v>
       </c>
     </row>
@@ -941,19 +961,19 @@
         <v>38</v>
       </c>
       <c r="I8" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F8:H8)=0,"NA",SUM(F8:H8))</f>
         <v>NA</v>
       </c>
       <c r="M8" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(J8:L8)=0,"NA",SUM(J8:L8))</f>
         <v>NA</v>
       </c>
       <c r="Q8" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(SUM(N8:P8)=0,"NA",SUM(N8:P8))</f>
         <v>NA</v>
       </c>
       <c r="U8" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R8:T8)=0,"NA",SUM(R8:T8))</f>
         <v>NA</v>
       </c>
       <c r="V8">
@@ -963,11 +983,11 @@
         <v>17</v>
       </c>
       <c r="Y8" s="3">
-        <f t="shared" si="5"/>
+        <f>IF(SUM(V8:X8)=0,"NA",SUM(V8:X8))</f>
         <v>36</v>
       </c>
       <c r="AC8" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z8:AB8)=0,"NA",SUM(Z8:AB8))</f>
         <v>NA</v>
       </c>
       <c r="AD8">
@@ -977,7 +997,7 @@
         <v>0</v>
       </c>
       <c r="AG8" s="3">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD8:AF8)=0,"NA",SUM(AD8:AF8))</f>
         <v>1</v>
       </c>
       <c r="AH8">
@@ -987,7 +1007,7 @@
         <v>17</v>
       </c>
       <c r="AK8" s="3">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH8:AJ8)=0,"NA",SUM(AH8:AJ8))</f>
         <v>37</v>
       </c>
     </row>
@@ -1009,35 +1029,35 @@
         <v>115</v>
       </c>
       <c r="I9" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F9:H9)=0,"NA",SUM(F9:H9))</f>
         <v>NA</v>
       </c>
       <c r="M9" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(J9:L9)=0,"NA",SUM(J9:L9))</f>
         <v>NA</v>
       </c>
       <c r="Q9" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(SUM(N9:P9)=0,"NA",SUM(N9:P9))</f>
         <v>NA</v>
       </c>
       <c r="U9" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R9:T9)=0,"NA",SUM(R9:T9))</f>
         <v>NA</v>
       </c>
       <c r="Y9" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(SUM(V9:X9)=0,"NA",SUM(V9:X9))</f>
         <v>NA</v>
       </c>
       <c r="AC9" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z9:AB9)=0,"NA",SUM(Z9:AB9))</f>
         <v>NA</v>
       </c>
       <c r="AG9" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD9:AF9)=0,"NA",SUM(AD9:AF9))</f>
         <v>NA</v>
       </c>
       <c r="AK9" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH9:AJ9)=0,"NA",SUM(AH9:AJ9))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1050,35 +1070,35 @@
         <v>NA</v>
       </c>
       <c r="I10" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F10:H10)=0,"NA",SUM(F10:H10))</f>
         <v>NA</v>
       </c>
       <c r="M10" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(J10:L10)=0,"NA",SUM(J10:L10))</f>
         <v>NA</v>
       </c>
       <c r="Q10" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(SUM(N10:P10)=0,"NA",SUM(N10:P10))</f>
         <v>NA</v>
       </c>
       <c r="U10" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R10:T10)=0,"NA",SUM(R10:T10))</f>
         <v>NA</v>
       </c>
       <c r="Y10" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(SUM(V10:X10)=0,"NA",SUM(V10:X10))</f>
         <v>NA</v>
       </c>
       <c r="AC10" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z10:AB10)=0,"NA",SUM(Z10:AB10))</f>
         <v>NA</v>
       </c>
       <c r="AG10" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD10:AF10)=0,"NA",SUM(AD10:AF10))</f>
         <v>NA</v>
       </c>
       <c r="AK10" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH10:AJ10)=0,"NA",SUM(AH10:AJ10))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1097,35 +1117,35 @@
         <v>256</v>
       </c>
       <c r="I11" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F11:H11)=0,"NA",SUM(F11:H11))</f>
         <v>NA</v>
       </c>
       <c r="M11" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(J11:L11)=0,"NA",SUM(J11:L11))</f>
         <v>NA</v>
       </c>
       <c r="Q11" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(SUM(N11:P11)=0,"NA",SUM(N11:P11))</f>
         <v>NA</v>
       </c>
       <c r="U11" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="U11:U17" si="1">IF(SUM(R11:T11)=0,"NA",SUM(R11:T11))</f>
         <v>NA</v>
       </c>
       <c r="Y11" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="Y11:Y16" si="2">IF(SUM(V11:X11)=0,"NA",SUM(V11:X11))</f>
         <v>NA</v>
       </c>
       <c r="AC11" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="AC11:AC16" si="3">IF(SUM(Z11:AB11)=0,"NA",SUM(Z11:AB11))</f>
         <v>NA</v>
       </c>
       <c r="AG11" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AG11:AG18" si="4">IF(SUM(AD11:AF11)=0,"NA",SUM(AD11:AF11))</f>
         <v>NA</v>
       </c>
       <c r="AK11" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH11:AJ11)=0,"NA",SUM(AH11:AJ11))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1144,35 +1164,35 @@
         <v>44</v>
       </c>
       <c r="I12" s="3" t="str">
+        <f>IF(SUM(F12:H12)=0,"NA",SUM(F12:H12))</f>
+        <v>NA</v>
+      </c>
+      <c r="M12" s="3" t="str">
+        <f>IF(SUM(J12:L12)=0,"NA",SUM(J12:L12))</f>
+        <v>NA</v>
+      </c>
+      <c r="Q12" s="3" t="str">
+        <f t="shared" ref="Q12:Q37" si="5">IF(SUM(N12:P12)=0,"NA",SUM(N12:P12))</f>
+        <v>NA</v>
+      </c>
+      <c r="U12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="M12" s="3" t="str">
+      <c r="Y12" s="3" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="Q12" s="3" t="str">
+      <c r="AC12" s="3" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
-      <c r="U12" s="3" t="str">
+      <c r="AG12" s="3" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="Y12" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>NA</v>
-      </c>
-      <c r="AC12" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG12" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
       <c r="AK12" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="AK12:AK18" si="6">IF(SUM(AH12:AJ12)=0,"NA",SUM(AH12:AJ12))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1180,46 +1200,40 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>190</v>
-      </c>
-      <c r="C13">
-        <v>187</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="0"/>
-        <v>377</v>
+      <c r="E13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
       </c>
       <c r="I13" s="3" t="str">
+        <f t="shared" ref="I13:I35" si="7">IF(SUM(F13:H13)=0,"NA",SUM(F13:H13))</f>
+        <v>NA</v>
+      </c>
+      <c r="M13" s="3" t="str">
+        <f t="shared" ref="M13:M36" si="8">IF(SUM(J13:L13)=0,"NA",SUM(J13:L13))</f>
+        <v>NA</v>
+      </c>
+      <c r="Q13" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="U13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="M13" s="3" t="str">
+      <c r="Y13" s="3" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="Q13" s="3" t="str">
+      <c r="AC13" s="3" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
-      <c r="U13" s="3" t="str">
+      <c r="AG13" s="3" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="Y13" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>NA</v>
-      </c>
-      <c r="AC13" s="3" t="str">
+      <c r="AK13" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG13" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-      <c r="AK13" s="3" t="str">
-        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
     </row>
@@ -1232,35 +1246,35 @@
         <v>NA</v>
       </c>
       <c r="I14" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="M14" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+      <c r="Q14" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="U14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="M14" s="3" t="str">
+      <c r="Y14" s="3" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="Q14" s="3" t="str">
+      <c r="AC14" s="3" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
-      <c r="U14" s="3" t="str">
+      <c r="AG14" s="3" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="Y14" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>NA</v>
-      </c>
-      <c r="AC14" s="3" t="str">
+      <c r="AK14" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG14" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-      <c r="AK14" s="3" t="str">
-        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
     </row>
@@ -1279,35 +1293,35 @@
         <v>119</v>
       </c>
       <c r="I15" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="M15" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+      <c r="Q15" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="U15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="M15" s="3" t="str">
+      <c r="Y15" s="3" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="Q15" s="3" t="str">
+      <c r="AC15" s="3" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
-      <c r="U15" s="3" t="str">
+      <c r="AG15" s="3" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="Y15" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>NA</v>
-      </c>
-      <c r="AC15" s="3" t="str">
+      <c r="AK15" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG15" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-      <c r="AK15" s="3" t="str">
-        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
     </row>
@@ -1326,35 +1340,35 @@
         <v>28</v>
       </c>
       <c r="I16" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="M16" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+      <c r="Q16" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="U16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="M16" s="3" t="str">
+      <c r="Y16" s="3" t="str">
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="Q16" s="3" t="str">
+      <c r="AC16" s="3" t="str">
         <f t="shared" si="3"/>
         <v>NA</v>
       </c>
-      <c r="U16" s="3" t="str">
+      <c r="AG16" s="3" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="Y16" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>NA</v>
-      </c>
-      <c r="AC16" s="3" t="str">
+      <c r="AK16" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG16" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-      <c r="AK16" s="3" t="str">
-        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
     </row>
@@ -1373,35 +1387,35 @@
         <v>48</v>
       </c>
       <c r="I17" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="M17" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+      <c r="Q17" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+      <c r="U17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>NA</v>
       </c>
-      <c r="M17" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>NA</v>
-      </c>
-      <c r="Q17" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-      <c r="U17" s="3" t="str">
+      <c r="Y17" s="3" t="str">
+        <f>IF(SUM(V17:X17)=0,"NA",SUM(V17:X17))</f>
+        <v>NA</v>
+      </c>
+      <c r="AC17" s="3" t="str">
+        <f>IF(SUM(Z17:AB17)=0,"NA",SUM(Z17:AB17))</f>
+        <v>NA</v>
+      </c>
+      <c r="AG17" s="3" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="Y17" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>NA</v>
-      </c>
-      <c r="AC17" s="3" t="str">
+      <c r="AK17" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG17" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-      <c r="AK17" s="3" t="str">
-        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
     </row>
@@ -1420,35 +1434,35 @@
         <v>294</v>
       </c>
       <c r="I18" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M18" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q18" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U18" s="3" t="str">
+        <f>IF(SUM(R18:T18)=0,"NA",SUM(R18:T18))</f>
+        <v>NA</v>
+      </c>
+      <c r="Y18" s="3" t="str">
+        <f>IF(SUM(V18:X18)=0,"NA",SUM(V18:X18))</f>
+        <v>NA</v>
+      </c>
+      <c r="AC18" s="3" t="str">
+        <f>IF(SUM(Z18:AB18)=0,"NA",SUM(Z18:AB18))</f>
+        <v>NA</v>
+      </c>
+      <c r="AG18" s="3" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="Y18" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>NA</v>
-      </c>
-      <c r="AC18" s="3" t="str">
+      <c r="AK18" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG18" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-      <c r="AK18" s="3" t="str">
-        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
     </row>
@@ -1461,35 +1475,35 @@
         <v>NA</v>
       </c>
       <c r="I19" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M19" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q19" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U19" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R19:T19)=0,"NA",SUM(R19:T19))</f>
         <v>NA</v>
       </c>
       <c r="Y19" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(SUM(V19:X19)=0,"NA",SUM(V19:X19))</f>
         <v>NA</v>
       </c>
       <c r="AC19" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z19:AB19)=0,"NA",SUM(Z19:AB19))</f>
         <v>NA</v>
       </c>
       <c r="AG19" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD19:AF19)=0,"NA",SUM(AD19:AF19))</f>
         <v>NA</v>
       </c>
       <c r="AK19" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH19:AJ19)=0,"NA",SUM(AH19:AJ19))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1508,35 +1522,35 @@
         <v>32</v>
       </c>
       <c r="I20" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M20" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q20" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R20:T20)=0,"NA",SUM(R20:T20))</f>
         <v>NA</v>
       </c>
       <c r="Y20" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(SUM(V20:X20)=0,"NA",SUM(V20:X20))</f>
         <v>NA</v>
       </c>
       <c r="AC20" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z20:AB20)=0,"NA",SUM(Z20:AB20))</f>
         <v>NA</v>
       </c>
       <c r="AG20" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD20:AF20)=0,"NA",SUM(AD20:AF20))</f>
         <v>NA</v>
       </c>
       <c r="AK20" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH20:AJ20)=0,"NA",SUM(AH20:AJ20))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1555,35 +1569,35 @@
         <v>37</v>
       </c>
       <c r="I21" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M21" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q21" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U21" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="U21:U43" si="9">IF(SUM(R21:T21)=0,"NA",SUM(R21:T21))</f>
         <v>NA</v>
       </c>
       <c r="Y21" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="Y21:Y55" si="10">IF(SUM(V21:X21)=0,"NA",SUM(V21:X21))</f>
         <v>NA</v>
       </c>
       <c r="AC21" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z21:AB21)=0,"NA",SUM(Z21:AB21))</f>
         <v>NA</v>
       </c>
       <c r="AG21" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD21:AF21)=0,"NA",SUM(AD21:AF21))</f>
         <v>NA</v>
       </c>
       <c r="AK21" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH21:AJ21)=0,"NA",SUM(AH21:AJ21))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1604,35 +1618,35 @@
         <v>1462</v>
       </c>
       <c r="I22" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M22" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q22" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U22" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y22" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC22" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z22:AB22)=0,"NA",SUM(Z22:AB22))</f>
         <v>NA</v>
       </c>
       <c r="AG22" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD22:AF22)=0,"NA",SUM(AD22:AF22))</f>
         <v>NA</v>
       </c>
       <c r="AK22" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH22:AJ22)=0,"NA",SUM(AH22:AJ22))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1644,37 +1658,58 @@
         <f t="shared" si="0"/>
         <v>NA</v>
       </c>
-      <c r="I23" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
-      </c>
-      <c r="M23" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>NA</v>
-      </c>
-      <c r="Q23" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-      <c r="U23" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>NA</v>
-      </c>
-      <c r="Y23" s="3" t="str">
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>146</v>
+      </c>
+      <c r="M23" s="3">
+        <f t="shared" si="8"/>
+        <v>146</v>
+      </c>
+      <c r="O23">
+        <v>8</v>
+      </c>
+      <c r="Q23" s="3">
         <f t="shared" si="5"/>
-        <v>NA</v>
+        <v>8</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="U23" s="3">
+        <f>IF(SUM(R23:T23)=0,"NA",SUM(R23:T23))</f>
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>103</v>
+      </c>
+      <c r="Y23" s="3">
+        <f>IF(SUM(V23:X23)=0,"NA",SUM(V23:X23))</f>
+        <v>103</v>
       </c>
       <c r="AC23" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG23" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-      <c r="AK23" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>NA</v>
+        <f>IF(SUM(Z23:AB23)=0,"NA",SUM(Z23:AB23))</f>
+        <v>NA</v>
+      </c>
+      <c r="AE23">
+        <v>11</v>
+      </c>
+      <c r="AG23" s="3">
+        <f>IF(SUM(AD23:AF23)=0,"NA",SUM(AD23:AF23))</f>
+        <v>11</v>
+      </c>
+      <c r="AI23">
+        <v>135</v>
+      </c>
+      <c r="AK23" s="3">
+        <f>IF(SUM(AH23:AJ23)=0,"NA",SUM(AH23:AJ23))</f>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -1692,35 +1727,35 @@
         <v>92</v>
       </c>
       <c r="I24" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M24" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q24" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U24" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y24" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC24" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="AC24:AC41" si="11">IF(SUM(Z24:AB24)=0,"NA",SUM(Z24:AB24))</f>
         <v>NA</v>
       </c>
       <c r="AG24" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AG24:AG40" si="12">IF(SUM(AD24:AF24)=0,"NA",SUM(AD24:AF24))</f>
         <v>NA</v>
       </c>
       <c r="AK24" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(SUM(AH24:AJ24)=0,"NA",SUM(AH24:AJ24))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1736,35 +1771,35 @@
         <v>50</v>
       </c>
       <c r="I25" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M25" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q25" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U25" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y25" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC25" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG25" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK25" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="AK25:AK54" si="13">IF(SUM(AH25:AJ25)=0,"NA",SUM(AH25:AJ25))</f>
         <v>NA</v>
       </c>
     </row>
@@ -1783,7 +1818,7 @@
         <v>55</v>
       </c>
       <c r="I26" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="J26">
@@ -1793,31 +1828,31 @@
         <v>22</v>
       </c>
       <c r="M26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="Q26" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U26" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y26" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC26" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG26" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK26" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -1836,31 +1871,31 @@
         <v>243</v>
       </c>
       <c r="I27" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M27" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q27" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U27" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y27" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC27" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG27" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AH27">
@@ -1870,7 +1905,7 @@
         <v>28</v>
       </c>
       <c r="AK27" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>243</v>
       </c>
     </row>
@@ -1883,35 +1918,35 @@
         <v>NA</v>
       </c>
       <c r="I28" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M28" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q28" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U28" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y28" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC28" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG28" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK28" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -1930,35 +1965,35 @@
         <v>120</v>
       </c>
       <c r="I29" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M29" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q29" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U29" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y29" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC29" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG29" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK29" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -1966,40 +2001,47 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="E30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="B30">
+        <f>460-184</f>
+        <v>276</v>
+      </c>
+      <c r="C30">
+        <v>184</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>460</v>
       </c>
       <c r="I30" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M30" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q30" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U30" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y30" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC30" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG30" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK30" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2018,35 +2060,35 @@
         <v>75</v>
       </c>
       <c r="I31" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M31" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q31" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U31" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y31" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC31" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG31" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK31" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2054,46 +2096,40 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>301</v>
-      </c>
-      <c r="C32">
-        <v>456</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="shared" si="0"/>
-        <v>757</v>
+      <c r="E32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
       </c>
       <c r="I32" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M32" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q32" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U32" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y32" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC32" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG32" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK32" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2112,35 +2148,35 @@
         <v>311</v>
       </c>
       <c r="I33" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M33" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q33" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U33" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y33" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC33" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG33" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK33" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2159,7 +2195,7 @@
         <v>154</v>
       </c>
       <c r="I34" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="J34">
@@ -2169,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="M34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="N34">
@@ -2179,11 +2215,11 @@
         <v>5</v>
       </c>
       <c r="Q34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="U34" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="V34">
@@ -2193,7 +2229,7 @@
         <v>77</v>
       </c>
       <c r="Y34" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>139</v>
       </c>
       <c r="Z34">
@@ -2203,7 +2239,7 @@
         <v>4</v>
       </c>
       <c r="AC34" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="AD34">
@@ -2213,7 +2249,7 @@
         <v>7</v>
       </c>
       <c r="AG34" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="AH34">
@@ -2223,7 +2259,7 @@
         <v>80</v>
       </c>
       <c r="AK34" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>146</v>
       </c>
     </row>
@@ -2236,35 +2272,35 @@
         <v>NA</v>
       </c>
       <c r="I35" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>NA</v>
       </c>
       <c r="M35" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q35" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U35" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y35" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC35" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG35" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK35" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2277,35 +2313,35 @@
         <v>NA</v>
       </c>
       <c r="I36" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F36:H36)=0,"NA",SUM(F36:H36))</f>
         <v>NA</v>
       </c>
       <c r="M36" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>NA</v>
       </c>
       <c r="Q36" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U36" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y36" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC36" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG36" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK36" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2324,35 +2360,35 @@
         <v>114</v>
       </c>
       <c r="I37" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F37:H37)=0,"NA",SUM(F37:H37))</f>
         <v>NA</v>
       </c>
       <c r="M37" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="M37:M53" si="14">IF(SUM(J37:L37)=0,"NA",SUM(J37:L37))</f>
         <v>NA</v>
       </c>
       <c r="Q37" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>NA</v>
       </c>
       <c r="U37" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y37" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC37" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG37" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK37" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2373,35 +2409,35 @@
         <v>606</v>
       </c>
       <c r="I38" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(SUM(F38:H38)=0,"NA",SUM(F38:H38))</f>
         <v>NA</v>
       </c>
       <c r="M38" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q38" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="Q38:Q54" si="15">IF(SUM(N38:P38)=0,"NA",SUM(N38:P38))</f>
         <v>NA</v>
       </c>
       <c r="U38" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y38" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC38" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG38" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK38" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2422,19 +2458,19 @@
         <v>2139</v>
       </c>
       <c r="I39" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I39:I56" si="16">IF(SUM(F39:H39)=0,"NA",SUM(F39:H39))</f>
         <v>NA</v>
       </c>
       <c r="M39" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q39" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U39" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="V39">
@@ -2444,19 +2480,19 @@
         <v>155</v>
       </c>
       <c r="Y39" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1522</v>
       </c>
       <c r="AC39" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG39" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK39" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2469,35 +2505,35 @@
         <v>NA</v>
       </c>
       <c r="I40" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M40" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q40" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U40" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y40" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC40" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG40" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>NA</v>
       </c>
       <c r="AK40" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2516,35 +2552,35 @@
         <v>99</v>
       </c>
       <c r="I41" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M41" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q41" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U41" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y41" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC41" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>NA</v>
       </c>
       <c r="AG41" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD41:AF41)=0,"NA",SUM(AD41:AF41))</f>
         <v>NA</v>
       </c>
       <c r="AK41" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2563,35 +2599,35 @@
         <v>235</v>
       </c>
       <c r="I42" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M42" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q42" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U42" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y42" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC42" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z42:AB42)=0,"NA",SUM(Z42:AB42))</f>
         <v>NA</v>
       </c>
       <c r="AG42" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD42:AF42)=0,"NA",SUM(AD42:AF42))</f>
         <v>NA</v>
       </c>
       <c r="AK42" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2611,35 +2647,35 @@
         <v>103</v>
       </c>
       <c r="I43" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M43" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q43" s="3" t="str">
-        <f>IF(SUM(N43:P43)=0,"NA",SUM(N43:P43))</f>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U43" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>NA</v>
       </c>
       <c r="Y43" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC43" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z43:AB43)=0,"NA",SUM(Z43:AB43))</f>
         <v>NA</v>
       </c>
       <c r="AG43" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(AD43:AF43)=0,"NA",SUM(AD43:AF43))</f>
         <v>NA</v>
       </c>
       <c r="AK43" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2655,50 +2691,50 @@
         <v>250</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>250</v>
       </c>
       <c r="L44">
         <v>7</v>
       </c>
       <c r="M44" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="P44">
         <v>372</v>
       </c>
       <c r="Q44" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>372</v>
       </c>
       <c r="U44" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(SUM(R44:T44)=0,"NA",SUM(R44:T44))</f>
         <v>NA</v>
       </c>
       <c r="X44">
         <v>235</v>
       </c>
       <c r="Y44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>235</v>
       </c>
       <c r="AC44" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(SUM(Z44:AB44)=0,"NA",SUM(Z44:AB44))</f>
         <v>NA</v>
       </c>
       <c r="AF44">
         <v>350</v>
       </c>
       <c r="AG44" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AG44:AG52" si="17">IF(SUM(AD44:AF44)=0,"NA",SUM(AD44:AF44))</f>
         <v>350</v>
       </c>
       <c r="AJ44">
         <v>473</v>
       </c>
       <c r="AK44" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>473</v>
       </c>
     </row>
@@ -2717,35 +2753,35 @@
         <v>127</v>
       </c>
       <c r="I45" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M45" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q45" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U45" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="U45:U54" si="18">IF(SUM(R45:T45)=0,"NA",SUM(R45:T45))</f>
         <v>NA</v>
       </c>
       <c r="Y45" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC45" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="AC45:AC53" si="19">IF(SUM(Z45:AB45)=0,"NA",SUM(Z45:AB45))</f>
         <v>NA</v>
       </c>
       <c r="AG45" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AK45" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2764,53 +2800,53 @@
         <v>64</v>
       </c>
       <c r="I46" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="L46">
         <v>4</v>
       </c>
       <c r="M46" s="3">
-        <f>IF(SUM(J46:L46)=0,"NA",SUM(J46:L46))</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="P46">
         <v>12</v>
       </c>
       <c r="Q46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="U46" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="X46">
         <v>34</v>
       </c>
       <c r="Y46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>34</v>
       </c>
       <c r="AB46">
         <v>5</v>
       </c>
       <c r="AC46" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
       <c r="AF46">
         <v>9</v>
       </c>
       <c r="AG46" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="AJ46">
         <v>50</v>
       </c>
       <c r="AK46" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
     </row>
@@ -2829,35 +2865,35 @@
         <v>70</v>
       </c>
       <c r="I47" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M47" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q47" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U47" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="Y47" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC47" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="AG47" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AK47" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2877,35 +2913,35 @@
         <v>252</v>
       </c>
       <c r="I48" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M48" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q48" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U48" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="Y48" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC48" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="AG48" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AK48" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2913,46 +2949,40 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49">
-        <v>375</v>
-      </c>
-      <c r="C49">
-        <v>384</v>
-      </c>
-      <c r="E49" s="3">
-        <f t="shared" si="0"/>
-        <v>759</v>
+      <c r="E49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
       </c>
       <c r="I49" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M49" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q49" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U49" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="Y49" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC49" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="AG49" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AK49" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -2971,35 +3001,35 @@
         <v>74</v>
       </c>
       <c r="I50" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>NA</v>
       </c>
       <c r="M50" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>NA</v>
       </c>
       <c r="Q50" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>NA</v>
       </c>
       <c r="U50" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>NA</v>
       </c>
       <c r="Y50" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>NA</v>
       </c>
       <c r="AC50" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="AG50" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>NA</v>
       </c>
       <c r="AK50" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>NA</v>
       </c>
     </row>
@@ -3007,54 +3037,318 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51">
+      <c r="E51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I51" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="M51" s="3" t="str">
+        <f>IF(SUM(J51:L51)=0,"NA",SUM(J51:L51))</f>
+        <v>NA</v>
+      </c>
+      <c r="Q51" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+      <c r="U51" s="3" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+      <c r="Y51" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>NA</v>
+      </c>
+      <c r="AC51" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="AG51" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="AK51" s="3" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52">
+        <v>190</v>
+      </c>
+      <c r="C52">
+        <v>187</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="0"/>
+        <v>377</v>
+      </c>
+      <c r="I52" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="M52" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>NA</v>
+      </c>
+      <c r="Q52" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+      <c r="U52" s="3" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+      <c r="Y52" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>NA</v>
+      </c>
+      <c r="AC52" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="AG52" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="AK52" s="3" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I53" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="M53" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>NA</v>
+      </c>
+      <c r="Q53" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+      <c r="U53" s="3" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+      <c r="Y53" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>NA</v>
+      </c>
+      <c r="AC53" s="3" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="AG53" s="3" t="str">
+        <f>IF(SUM(AD53:AF53)=0,"NA",SUM(AD53:AF53))</f>
+        <v>NA</v>
+      </c>
+      <c r="AK53" s="3" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+      <c r="I54" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="M54" s="3" t="str">
+        <f>IF(SUM(J54:L54)=0,"NA",SUM(J54:L54))</f>
+        <v>NA</v>
+      </c>
+      <c r="Q54" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+      <c r="U54" s="3" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+      <c r="Y54" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>NA</v>
+      </c>
+      <c r="AC54" s="3" t="str">
+        <f>IF(SUM(Z54:AB54)=0,"NA",SUM(Z54:AB54))</f>
+        <v>NA</v>
+      </c>
+      <c r="AG54" s="3" t="str">
+        <f>IF(SUM(AD54:AF54)=0,"NA",SUM(AD54:AF54))</f>
+        <v>NA</v>
+      </c>
+      <c r="AK54" s="3" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55">
+        <v>301</v>
+      </c>
+      <c r="C55">
+        <v>456</v>
+      </c>
+      <c r="E55" s="3">
+        <f>IF(SUM(B55:D55)=0,"NA",SUM(B55:D55))</f>
+        <v>757</v>
+      </c>
+      <c r="I55" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="M55" s="3" t="str">
+        <f>IF(SUM(J55:L55)=0,"NA",SUM(J55:L55))</f>
+        <v>NA</v>
+      </c>
+      <c r="Q55" s="3" t="str">
+        <f>IF(SUM(N55:P55)=0,"NA",SUM(N55:P55))</f>
+        <v>NA</v>
+      </c>
+      <c r="U55" s="3" t="str">
+        <f>IF(SUM(R55:T55)=0,"NA",SUM(R55:T55))</f>
+        <v>NA</v>
+      </c>
+      <c r="Y55" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>NA</v>
+      </c>
+      <c r="AC55" s="3" t="str">
+        <f>IF(SUM(Z55:AB55)=0,"NA",SUM(Z55:AB55))</f>
+        <v>NA</v>
+      </c>
+      <c r="AG55" s="3" t="str">
+        <f>IF(SUM(AD55:AF55)=0,"NA",SUM(AD55:AF55))</f>
+        <v>NA</v>
+      </c>
+      <c r="AK55" s="3" t="str">
+        <f>IF(SUM(AH55:AJ55)=0,"NA",SUM(AH55:AJ55))</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56">
+        <v>375</v>
+      </c>
+      <c r="C56">
+        <v>384</v>
+      </c>
+      <c r="E56" s="3">
+        <f>IF(SUM(B56:D56)=0,"NA",SUM(B56:D56))</f>
+        <v>759</v>
+      </c>
+      <c r="I56" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="M56" s="3" t="str">
+        <f>IF(SUM(J56:L56)=0,"NA",SUM(J56:L56))</f>
+        <v>NA</v>
+      </c>
+      <c r="Q56" s="3" t="str">
+        <f>IF(SUM(N56:P56)=0,"NA",SUM(N56:P56))</f>
+        <v>NA</v>
+      </c>
+      <c r="U56" s="3" t="str">
+        <f>IF(SUM(R56:T56)=0,"NA",SUM(R56:T56))</f>
+        <v>NA</v>
+      </c>
+      <c r="Y56" s="3" t="str">
+        <f>IF(SUM(V56:X56)=0,"NA",SUM(V56:X56))</f>
+        <v>NA</v>
+      </c>
+      <c r="AC56" s="3" t="str">
+        <f>IF(SUM(Z56:AB56)=0,"NA",SUM(Z56:AB56))</f>
+        <v>NA</v>
+      </c>
+      <c r="AG56" s="3" t="str">
+        <f>IF(SUM(AD56:AF56)=0,"NA",SUM(AD56:AF56))</f>
+        <v>NA</v>
+      </c>
+      <c r="AK56" s="3" t="str">
+        <f>IF(SUM(AH56:AJ56)=0,"NA",SUM(AH56:AJ56))</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57">
         <v>76</v>
       </c>
-      <c r="C51">
+      <c r="C57">
         <v>161</v>
       </c>
-      <c r="E51" s="3">
-        <f t="shared" si="0"/>
+      <c r="E57" s="3">
+        <f>IF(SUM(B57:D57)=0,"NA",SUM(B57:D57))</f>
         <v>237</v>
       </c>
-      <c r="I51" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>NA</v>
-      </c>
-      <c r="M51" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>NA</v>
-      </c>
-      <c r="Q51" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-      <c r="U51" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>NA</v>
-      </c>
-      <c r="Y51" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>NA</v>
-      </c>
-      <c r="AC51" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="AG51" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-      <c r="AK51" s="3" t="str">
-        <f t="shared" si="8"/>
+      <c r="I57" s="3" t="str">
+        <f>IF(SUM(F57:H57)=0,"NA",SUM(F57:H57))</f>
+        <v>NA</v>
+      </c>
+      <c r="M57" s="3" t="str">
+        <f>IF(SUM(J57:L57)=0,"NA",SUM(J57:L57))</f>
+        <v>NA</v>
+      </c>
+      <c r="Q57" s="3" t="str">
+        <f>IF(SUM(N57:P57)=0,"NA",SUM(N57:P57))</f>
+        <v>NA</v>
+      </c>
+      <c r="U57" s="3" t="str">
+        <f>IF(SUM(R57:T57)=0,"NA",SUM(R57:T57))</f>
+        <v>NA</v>
+      </c>
+      <c r="Y57" s="3" t="str">
+        <f>IF(SUM(V57:X57)=0,"NA",SUM(V57:X57))</f>
+        <v>NA</v>
+      </c>
+      <c r="AC57" s="3" t="str">
+        <f>IF(SUM(Z57:AB57)=0,"NA",SUM(Z57:AB57))</f>
+        <v>NA</v>
+      </c>
+      <c r="AG57" s="3" t="str">
+        <f>IF(SUM(AD57:AF57)=0,"NA",SUM(AD57:AF57))</f>
+        <v>NA</v>
+      </c>
+      <c r="AK57" s="3" t="str">
+        <f>IF(SUM(AH57:AJ57)=0,"NA",SUM(AH57:AJ57))</f>
         <v>NA</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AK57">
+    <sortCondition ref="A2:A57"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="E2" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
clean the new dataset
still have naming issue with meta_data_comparison
</commit_message>
<xml_diff>
--- a/cleaned_data/Meta_data_demo.xlsx
+++ b/cleaned_data/Meta_data_demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syl05\OneDrive\Desktop\UMICH\Summer 2025\RCT_Reseach\cleaned_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8951E211-6C15-41FA-AEC1-1EED4D1BBE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BF74F8-F5BB-460D-A491-5EAD1CEA2CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,10 +517,10 @@
   <dimension ref="A1:AK57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H38" sqref="H38"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,14 +2138,14 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C33">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="E33" s="3">
         <f t="shared" si="8"/>
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="I33" s="3" t="str">
         <f t="shared" si="15"/>

</xml_diff>